<commit_message>
ERS requisitos de agente de playa en raiz
</commit_message>
<xml_diff>
--- a/Excel/Infracciones.xlsx
+++ b/Excel/Infracciones.xlsx
@@ -1,14 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\playa\asd\sugpaDoc\Excel\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="84" windowWidth="22068" windowHeight="9480"/>
+    <workbookView xWindow="480" yWindow="90" windowWidth="22065" windowHeight="9480" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
-    <sheet name="Hoja2" sheetId="2" r:id="rId2"/>
+    <sheet name="codigos" sheetId="1" r:id="rId1"/>
+    <sheet name="tipos infraccion" sheetId="2" r:id="rId2"/>
     <sheet name="Hoja3" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="124519"/>
@@ -16,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="269" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="159">
   <si>
     <t>Código</t>
   </si>
@@ -498,8 +503,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -549,6 +554,14 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -595,7 +608,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -627,9 +640,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -661,6 +675,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -836,21 +851,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C134"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A104" workbookViewId="0">
-      <selection activeCell="C134" sqref="C134"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C47" sqref="C47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="27.77734375" style="2" customWidth="1"/>
-    <col min="2" max="2" width="7.77734375" style="2" customWidth="1"/>
-    <col min="3" max="3" width="169.21875" customWidth="1"/>
+    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
+    <col min="2" max="2" width="7.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="169.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
@@ -861,7 +876,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:3">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
@@ -872,7 +887,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="3" spans="1:3">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>3</v>
       </c>
@@ -883,7 +898,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:3">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -894,7 +909,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:3">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -905,7 +920,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="6" spans="1:3">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -916,7 +931,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:3">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>4</v>
       </c>
@@ -927,7 +942,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="8" spans="1:3">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
@@ -938,7 +953,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="9" spans="1:3">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>5</v>
       </c>
@@ -949,7 +964,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>5</v>
       </c>
@@ -960,7 +975,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="11" spans="1:3">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>5</v>
       </c>
@@ -971,7 +986,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="12" spans="1:3">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>5</v>
       </c>
@@ -982,7 +997,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="13" spans="1:3">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>5</v>
       </c>
@@ -993,7 +1008,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:3">
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>6</v>
       </c>
@@ -1004,7 +1019,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="15" spans="1:3">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>6</v>
       </c>
@@ -1015,7 +1030,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>7</v>
       </c>
@@ -1026,7 +1041,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:3">
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>7</v>
       </c>
@@ -1037,7 +1052,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:3">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>7</v>
       </c>
@@ -1048,7 +1063,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:3">
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>7</v>
       </c>
@@ -1059,7 +1074,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:3">
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>7</v>
       </c>
@@ -1070,7 +1085,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="21" spans="1:3">
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>8</v>
       </c>
@@ -1081,7 +1096,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="22" spans="1:3">
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>8</v>
       </c>
@@ -1092,7 +1107,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="23" spans="1:3">
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>8</v>
       </c>
@@ -1103,7 +1118,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="24" spans="1:3">
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>8</v>
       </c>
@@ -1114,7 +1129,7 @@
         <v>48</v>
       </c>
     </row>
-    <row r="25" spans="1:3">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>9</v>
       </c>
@@ -1125,7 +1140,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="26" spans="1:3">
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>9</v>
       </c>
@@ -1136,7 +1151,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="27" spans="1:3">
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>10</v>
       </c>
@@ -1147,7 +1162,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="28" spans="1:3">
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>10</v>
       </c>
@@ -1158,7 +1173,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="29" spans="1:3">
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>10</v>
       </c>
@@ -1169,7 +1184,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="30" spans="1:3">
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>10</v>
       </c>
@@ -1180,7 +1195,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="31" spans="1:3">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>10</v>
       </c>
@@ -1191,7 +1206,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="32" spans="1:3">
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>10</v>
       </c>
@@ -1202,7 +1217,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="33" spans="1:3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>10</v>
       </c>
@@ -1213,7 +1228,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="34" spans="1:3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>11</v>
       </c>
@@ -1224,7 +1239,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>13</v>
       </c>
@@ -1235,7 +1250,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="36" spans="1:3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>13</v>
       </c>
@@ -1246,7 +1261,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="37" spans="1:3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>13</v>
       </c>
@@ -1257,7 +1272,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>13</v>
       </c>
@@ -1268,7 +1283,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="39" spans="1:3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>13</v>
       </c>
@@ -1279,7 +1294,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="40" spans="1:3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>13</v>
       </c>
@@ -1290,7 +1305,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="41" spans="1:3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>13</v>
       </c>
@@ -1301,7 +1316,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="42" spans="1:3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>13</v>
       </c>
@@ -1312,7 +1327,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="43" spans="1:3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>13</v>
       </c>
@@ -1323,7 +1338,7 @@
         <v>66</v>
       </c>
     </row>
-    <row r="44" spans="1:3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>13</v>
       </c>
@@ -1334,7 +1349,7 @@
         <v>67</v>
       </c>
     </row>
-    <row r="45" spans="1:3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>14</v>
       </c>
@@ -1345,7 +1360,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="46" spans="1:3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>14</v>
       </c>
@@ -1356,7 +1371,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="47" spans="1:3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>15</v>
       </c>
@@ -1367,7 +1382,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="48" spans="1:3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>15</v>
       </c>
@@ -1378,7 +1393,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="49" spans="1:3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>16</v>
       </c>
@@ -1389,7 +1404,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="50" spans="1:3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>16</v>
       </c>
@@ -1400,7 +1415,7 @@
         <v>73</v>
       </c>
     </row>
-    <row r="51" spans="1:3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>16</v>
       </c>
@@ -1411,7 +1426,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>17</v>
       </c>
@@ -1422,7 +1437,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="53" spans="1:3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>18</v>
       </c>
@@ -1433,7 +1448,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="54" spans="1:3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>19</v>
       </c>
@@ -1444,7 +1459,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="55" spans="1:3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>19</v>
       </c>
@@ -1455,7 +1470,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="56" spans="1:3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>19</v>
       </c>
@@ -1466,7 +1481,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="57" spans="1:3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>19</v>
       </c>
@@ -1477,7 +1492,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="58" spans="1:3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>19</v>
       </c>
@@ -1488,7 +1503,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="59" spans="1:3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>19</v>
       </c>
@@ -1499,7 +1514,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="60" spans="1:3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>19</v>
       </c>
@@ -1510,7 +1525,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="61" spans="1:3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>19</v>
       </c>
@@ -1521,7 +1536,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="62" spans="1:3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>19</v>
       </c>
@@ -1532,7 +1547,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="63" spans="1:3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>19</v>
       </c>
@@ -1543,7 +1558,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="64" spans="1:3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>19</v>
       </c>
@@ -1554,7 +1569,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="65" spans="1:3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>19</v>
       </c>
@@ -1565,7 +1580,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="66" spans="1:3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>19</v>
       </c>
@@ -1576,7 +1591,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="67" spans="1:3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>19</v>
       </c>
@@ -1587,7 +1602,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="68" spans="1:3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>19</v>
       </c>
@@ -1598,7 +1613,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="69" spans="1:3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>19</v>
       </c>
@@ -1609,7 +1624,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="70" spans="1:3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>19</v>
       </c>
@@ -1620,7 +1635,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="71" spans="1:3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>19</v>
       </c>
@@ -1631,7 +1646,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="72" spans="1:3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>19</v>
       </c>
@@ -1642,7 +1657,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="73" spans="1:3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>19</v>
       </c>
@@ -1653,7 +1668,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="74" spans="1:3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>19</v>
       </c>
@@ -1664,7 +1679,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="75" spans="1:3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>20</v>
       </c>
@@ -1675,7 +1690,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="76" spans="1:3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>20</v>
       </c>
@@ -1686,7 +1701,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="77" spans="1:3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>21</v>
       </c>
@@ -1697,7 +1712,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="78" spans="1:3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>21</v>
       </c>
@@ -1708,7 +1723,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="79" spans="1:3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>21</v>
       </c>
@@ -1719,7 +1734,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="80" spans="1:3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>21</v>
       </c>
@@ -1730,7 +1745,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="81" spans="1:3">
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>21</v>
       </c>
@@ -1741,7 +1756,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="82" spans="1:3">
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>21</v>
       </c>
@@ -1752,7 +1767,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="83" spans="1:3">
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>21</v>
       </c>
@@ -1763,7 +1778,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="84" spans="1:3">
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>21</v>
       </c>
@@ -1774,7 +1789,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="85" spans="1:3">
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>21</v>
       </c>
@@ -1785,7 +1800,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="86" spans="1:3">
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>21</v>
       </c>
@@ -1796,7 +1811,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="87" spans="1:3">
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>21</v>
       </c>
@@ -1807,7 +1822,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="88" spans="1:3">
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>21</v>
       </c>
@@ -1818,7 +1833,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="89" spans="1:3">
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>21</v>
       </c>
@@ -1829,7 +1844,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="90" spans="1:3">
+    <row r="90" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>21</v>
       </c>
@@ -1840,7 +1855,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="91" spans="1:3">
+    <row r="91" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>21</v>
       </c>
@@ -1851,7 +1866,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="92" spans="1:3">
+    <row r="92" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>21</v>
       </c>
@@ -1862,7 +1877,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="93" spans="1:3">
+    <row r="93" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>21</v>
       </c>
@@ -1873,7 +1888,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="94" spans="1:3">
+    <row r="94" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>21</v>
       </c>
@@ -1884,7 +1899,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="95" spans="1:3">
+    <row r="95" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>21</v>
       </c>
@@ -1895,7 +1910,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="96" spans="1:3">
+    <row r="96" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>21</v>
       </c>
@@ -1906,7 +1921,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="97" spans="1:3">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>21</v>
       </c>
@@ -1917,7 +1932,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="98" spans="1:3">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>21</v>
       </c>
@@ -1928,7 +1943,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="99" spans="1:3">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>116</v>
       </c>
@@ -1939,7 +1954,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="100" spans="1:3">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>116</v>
       </c>
@@ -1950,7 +1965,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="101" spans="1:3">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>116</v>
       </c>
@@ -1961,7 +1976,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="102" spans="1:3">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>116</v>
       </c>
@@ -1972,7 +1987,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="103" spans="1:3">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>116</v>
       </c>
@@ -1983,7 +1998,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="104" spans="1:3">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>116</v>
       </c>
@@ -1994,7 +2009,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="105" spans="1:3">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>116</v>
       </c>
@@ -2005,7 +2020,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="106" spans="1:3">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>116</v>
       </c>
@@ -2016,7 +2031,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="107" spans="1:3">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>116</v>
       </c>
@@ -2027,7 +2042,7 @@
         <v>131</v>
       </c>
     </row>
-    <row r="108" spans="1:3">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>116</v>
       </c>
@@ -2038,7 +2053,7 @@
         <v>133</v>
       </c>
     </row>
-    <row r="109" spans="1:3">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>116</v>
       </c>
@@ -2049,7 +2064,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="110" spans="1:3">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>116</v>
       </c>
@@ -2060,7 +2075,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="111" spans="1:3">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>116</v>
       </c>
@@ -2071,7 +2086,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="112" spans="1:3">
+    <row r="112" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>116</v>
       </c>
@@ -2082,7 +2097,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="113" spans="1:3">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>116</v>
       </c>
@@ -2093,7 +2108,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="114" spans="1:3">
+    <row r="114" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>22</v>
       </c>
@@ -2104,7 +2119,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="115" spans="1:3">
+    <row r="115" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>22</v>
       </c>
@@ -2115,7 +2130,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="116" spans="1:3">
+    <row r="116" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>22</v>
       </c>
@@ -2126,7 +2141,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="117" spans="1:3">
+    <row r="117" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>22</v>
       </c>
@@ -2137,7 +2152,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="118" spans="1:3">
+    <row r="118" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>22</v>
       </c>
@@ -2148,7 +2163,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="119" spans="1:3">
+    <row r="119" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>22</v>
       </c>
@@ -2159,7 +2174,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="120" spans="1:3">
+    <row r="120" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>22</v>
       </c>
@@ -2170,7 +2185,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="121" spans="1:3">
+    <row r="121" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>22</v>
       </c>
@@ -2181,7 +2196,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="122" spans="1:3">
+    <row r="122" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>22</v>
       </c>
@@ -2192,7 +2207,7 @@
         <v>146</v>
       </c>
     </row>
-    <row r="123" spans="1:3">
+    <row r="123" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>22</v>
       </c>
@@ -2203,7 +2218,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="124" spans="1:3">
+    <row r="124" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>22</v>
       </c>
@@ -2214,7 +2229,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="125" spans="1:3">
+    <row r="125" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>22</v>
       </c>
@@ -2225,7 +2240,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="126" spans="1:3">
+    <row r="126" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>23</v>
       </c>
@@ -2236,7 +2251,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="127" spans="1:3">
+    <row r="127" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>23</v>
       </c>
@@ -2247,7 +2262,7 @@
         <v>151</v>
       </c>
     </row>
-    <row r="128" spans="1:3">
+    <row r="128" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>23</v>
       </c>
@@ -2258,7 +2273,7 @@
         <v>152</v>
       </c>
     </row>
-    <row r="129" spans="1:3">
+    <row r="129" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>23</v>
       </c>
@@ -2269,7 +2284,7 @@
         <v>153</v>
       </c>
     </row>
-    <row r="130" spans="1:3">
+    <row r="130" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>24</v>
       </c>
@@ -2280,7 +2295,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="131" spans="1:3">
+    <row r="131" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>24</v>
       </c>
@@ -2291,7 +2306,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="132" spans="1:3">
+    <row r="132" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>24</v>
       </c>
@@ -2302,7 +2317,7 @@
         <v>156</v>
       </c>
     </row>
-    <row r="133" spans="1:3">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>24</v>
       </c>
@@ -2313,7 +2328,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="134" spans="1:3">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>25</v>
       </c>
@@ -2331,24 +2346,150 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A97"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
-  <sheetData/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A38" s="2" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A40" s="2" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A62" s="2" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="2" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A89" s="2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A93" s="2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A97" s="2" t="s">
+        <v>25</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Actualizo raiz, infracciones resumidas, excel para cargar la base
</commit_message>
<xml_diff>
--- a/Excel/Infracciones.xlsx
+++ b/Excel/Infracciones.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="293" uniqueCount="159">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="313" uniqueCount="179">
   <si>
     <t>Código</t>
   </si>
@@ -498,6 +498,66 @@
   </si>
   <si>
     <t>Prohibición circular según DÍA/HORA/CARACTERÍSTICA vehíc.</t>
+  </si>
+  <si>
+    <t>Abreviacion</t>
+  </si>
+  <si>
+    <t>ALCO</t>
+  </si>
+  <si>
+    <t>BARR</t>
+  </si>
+  <si>
+    <t>CARR</t>
+  </si>
+  <si>
+    <t>CELU</t>
+  </si>
+  <si>
+    <t>COND</t>
+  </si>
+  <si>
+    <t>DOCU</t>
+  </si>
+  <si>
+    <t>ENSE</t>
+  </si>
+  <si>
+    <t>ESTA</t>
+  </si>
+  <si>
+    <t>INDI</t>
+  </si>
+  <si>
+    <t>LICE</t>
+  </si>
+  <si>
+    <t>LUCE</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LUZ </t>
+  </si>
+  <si>
+    <t>MOTO</t>
+  </si>
+  <si>
+    <t>PEAT</t>
+  </si>
+  <si>
+    <t>PRIN</t>
+  </si>
+  <si>
+    <t>SEGU</t>
+  </si>
+  <si>
+    <t>ALCO-DOC-LICE</t>
+  </si>
+  <si>
+    <t>Alcoholemia y otras Negativo</t>
+  </si>
+  <si>
+    <t>ALCN</t>
   </si>
 </sst>
 </file>
@@ -855,7 +915,7 @@
   <dimension ref="A1:C134"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C47" sqref="C47"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2347,10 +2407,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A97"/>
+  <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2358,89 +2418,151 @@
     <col min="1" max="1" width="27.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D2" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="B3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" s="2" t="s">
+      <c r="B4" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" s="2" t="s">
+      <c r="B5" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" s="2" t="s">
+      <c r="B6" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" s="2" t="s">
+      <c r="B7" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A8" s="2" t="s">
+      <c r="B8" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="9" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A9" s="2" t="s">
+      <c r="B9" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="10" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A10" s="2" t="s">
+      <c r="B10" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A11" s="2" t="s">
+      <c r="B11" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="2" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="12" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A12" s="2" t="s">
+      <c r="B12" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" s="2" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="13" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A13" s="2" t="s">
+      <c r="B13" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="14" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A14" s="2" t="s">
+      <c r="B14" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="15" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A15" s="2" t="s">
+      <c r="B15" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="16" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A16" s="2" t="s">
+      <c r="B16" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A17" s="2" t="s">
+      <c r="B17" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A18" s="2" t="s">
         <v>19</v>
+      </c>
+      <c r="B18" t="s">
+        <v>175</v>
       </c>
     </row>
     <row r="38" spans="1:1" x14ac:dyDescent="0.25">

</xml_diff>